<commit_message>
Updates to code to integrate Maurice's suggestions
Modified site-level corallivory intensity in response to coral cover and parrtofish density models.
</commit_message>
<xml_diff>
--- a/supplements/Formatted Supplemental Tables.xlsx
+++ b/supplements/Formatted Supplemental Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahrempel/My Drive/Research_Archives/ecological_drivers_corallivory/supplements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C63E410-D891-9244-9088-F6216CBA6021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BDCFCE-235A-2A48-8FE9-E9A6BAD7A301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="500" windowWidth="22540" windowHeight="16620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="500" windowWidth="22540" windowHeight="16620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_S1" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="162">
   <si>
     <t>Region</t>
   </si>
@@ -261,9 +261,6 @@
     <t>&lt;0.001</t>
   </si>
   <si>
-    <t>Corallivore density</t>
-  </si>
-  <si>
     <t>Coral cover (%)</t>
   </si>
   <si>
@@ -322,24 +319,6 @@
   </si>
   <si>
     <t>[0.283, 0.840]</t>
-  </si>
-  <si>
-    <t>[-1.367, 3.054]</t>
-  </si>
-  <si>
-    <t>[-7.827, -3.149]</t>
-  </si>
-  <si>
-    <t>[0.049, 0.681]</t>
-  </si>
-  <si>
-    <t>[-0.061, 0.056]</t>
-  </si>
-  <si>
-    <t>[-0.160, 0.437]</t>
-  </si>
-  <si>
-    <t>[-0.080, 0.027]</t>
   </si>
   <si>
     <t>[-7.752, -4.521]</t>
@@ -688,6 +667,36 @@
   <si>
     <t>[0.030, 1.493]</t>
   </si>
+  <si>
+    <t>[-1.295, 2.937]</t>
+  </si>
+  <si>
+    <t>[-0.134, 0.556]</t>
+  </si>
+  <si>
+    <t>[-0.075, 0.052]</t>
+  </si>
+  <si>
+    <t>[-0.029, 0.011]</t>
+  </si>
+  <si>
+    <t>[-7.703, -3.274]</t>
+  </si>
+  <si>
+    <t>[0.048, 0.785]</t>
+  </si>
+  <si>
+    <t>[-0.061, 0.075]</t>
+  </si>
+  <si>
+    <t>[-0.029, 0.016]</t>
+  </si>
+  <si>
+    <t>√(Corallivore density)</t>
+  </si>
+  <si>
+    <t>√(Corallivore density) x (coral cover)</t>
+  </si>
 </sst>
 </file>
 
@@ -698,7 +707,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -835,13 +844,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1290,153 +1292,158 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="22" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="22" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1814,542 +1821,542 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="27" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="33">
         <v>9.2684440000000006</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="33">
         <v>-82.241917000000001</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="21">
         <v>2</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="34">
         <v>9.3594439999999999</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="34">
         <v>-82.276667000000003</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>2</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="33">
         <v>9.2147780000000008</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="33">
         <v>-82.324556000000001</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="21">
         <v>2</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="34">
         <v>9.2438330000000004</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="34">
         <v>-82.145139</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>2</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="33">
         <v>9.2883060000000004</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="33">
         <v>-82.256777999999997</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="21">
         <v>2</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="34">
         <v>9.2346939999999993</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="34">
         <v>-82.345528000000002</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>2</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="33">
         <v>9.24</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="33">
         <v>-82.337500000000006</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="21">
         <v>2</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="34">
         <v>9.2712500000000002</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="34">
         <v>-82.298056000000003</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>2</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="33">
         <v>9.3488059999999997</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="33">
         <v>-82.262861000000001</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="21">
         <v>2</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="36">
         <v>9.2891940000000002</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="36">
         <v>-82.295693999999997</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="35">
         <v>2</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="35">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="33">
         <v>24.961189999999998</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="33">
         <v>-80.456647000000004</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="21">
         <v>2</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="37">
         <v>24.927060000000001</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="37">
         <v>-80.505504999999999</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="30">
         <v>3</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="33">
         <v>25.03482</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="33">
         <v>-80.347778000000005</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="21">
         <v>4</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="21">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="39">
         <v>25.008469999999999</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="39">
         <v>-80.376266000000001</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="38">
         <v>2</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="38">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="33">
         <v>17.787870000000002</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="33">
         <v>-64.609954999999999</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="21">
         <v>11</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="34">
         <v>17.786709999999999</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="34">
         <v>-64.608797999999993</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>23</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="33">
         <v>17.789390000000001</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="33">
         <v>-64.610279000000006</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="21">
         <v>8</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="34">
         <v>17.77308</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="34">
         <v>-64.812824000000006</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="11">
         <v>32</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="33">
         <v>17.761479999999999</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="33">
         <v>-64.720011999999997</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="21">
         <v>30</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="21">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="34">
         <v>17.768439999999998</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="34">
         <v>-64.823126000000002</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="11">
         <v>27</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="33">
         <v>17.779879999999999</v>
       </c>
-      <c r="D22" s="37">
+      <c r="D22" s="33">
         <v>-64.760394000000005</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="21">
         <v>19</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="21">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="36">
         <v>17.761119999999998</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="36">
         <v>-64.607426000000004</v>
       </c>
-      <c r="E23" s="39">
+      <c r="E23" s="35">
         <v>25</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="35">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="33">
         <v>12.125730000000001</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="33">
         <v>-68.288225999999995</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="21">
         <v>7</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="37">
         <v>12.17428</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="37">
         <v>-68.290726000000006</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="30">
         <v>5</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="33">
         <v>12.21912</v>
       </c>
-      <c r="D26" s="37">
+      <c r="D26" s="33">
         <v>-68.352683999999996</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="21">
         <v>26</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="41">
         <v>12.21496</v>
       </c>
-      <c r="D27" s="45">
+      <c r="D27" s="41">
         <v>-68.337958</v>
       </c>
-      <c r="E27" s="44">
+      <c r="E27" s="40">
         <v>32</v>
       </c>
-      <c r="F27" s="44">
+      <c r="F27" s="40">
         <v>8</v>
       </c>
     </row>
@@ -2373,178 +2380,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>122</v>
+      <c r="C1" s="27" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="25">
+      <c r="A2" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="21">
         <v>74</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="28">
         <v>22.6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>73</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>22.3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="21">
         <v>59</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="21">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>57</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>17.399999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="21">
         <v>12</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="21">
         <v>3.7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>11</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>3.4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="21">
         <v>9</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="21">
         <v>2.8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>9</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>2.8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="21">
         <v>8</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="21">
         <v>2.4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>5</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="21">
         <v>3</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="21">
         <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="30">
         <v>3</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="30">
         <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="21">
         <v>2</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="21">
         <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="30">
         <v>1</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="30">
         <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="32">
         <v>1</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16" s="32">
         <v>0.3</v>
       </c>
     </row>
@@ -2575,123 +2582,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="21">
         <v>2.38</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="21">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>1.85</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="21">
         <v>1.02</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="21">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>0.92</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="21">
         <v>0.37</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="21">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>0.26</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="21">
         <v>0.02</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="21">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="22">
         <v>0</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="23">
         <v>0</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="21">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="25">
         <v>0</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="26">
         <v>45</v>
       </c>
     </row>
@@ -2702,170 +2709,202 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1162ECB6-7014-2547-9AF5-E86990302D6E}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="7.5" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="44" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6">
-        <v>0.748</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>94</v>
+      <c r="C2" s="50">
+        <v>0.76</v>
+      </c>
+      <c r="D2" s="50">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E2" s="50">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="48">
+        <v>1.1990000000000001</v>
+      </c>
+      <c r="D3" s="48">
+        <v>0.23</v>
+      </c>
+      <c r="E3" s="48">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="9">
-        <v>0.90900000000000003</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="C4" s="46">
+        <v>-0.36299999999999999</v>
+      </c>
+      <c r="D4" s="46">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="E4" s="46">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="22">
-        <v>-0.97799999999999998</v>
-      </c>
-      <c r="D4" s="22">
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="E4" s="22">
-        <v>-2.7E-2</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="51">
+        <v>-0.84799999999999998</v>
+      </c>
+      <c r="D5" s="51">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E5" s="51">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="9">
-        <v>-4.5979999999999999</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C6" s="50">
+        <v>-4.859</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E6" s="50">
         <v>-5.4880000000000004</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="F6" s="49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="48">
+        <v>2.2160000000000002</v>
+      </c>
+      <c r="D7" s="48">
+        <v>2.7E-2</v>
+      </c>
+      <c r="E7" s="48">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="6">
-        <v>2.262</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2.4E-2</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="23">
-        <v>-9.2999999999999999E-2</v>
-      </c>
-      <c r="D7" s="23">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="E7" s="23">
-        <v>-3.0000000000000001E-3</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="49">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="D8" s="49">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="E8" s="49">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="51">
+        <v>-0.54700000000000004</v>
+      </c>
+      <c r="D9" s="51">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E9" s="51">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2891,283 +2930,283 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>-0.996</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>0.31900000000000001</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>-0.746</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="8">
+        <v>-1.6759999999999999</v>
+      </c>
+      <c r="D3" s="6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>-0.86399999999999999</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-2.532</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-1.2549999999999999</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="8">
+        <v>-3.2519999999999998</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>-1.38</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5.524</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2.177</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>-2.81</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E7" s="12">
+        <v>-1.0529999999999999</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3.008</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.47</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="9">
-        <v>-1.6759999999999999</v>
-      </c>
-      <c r="D3" s="7">
-        <v>9.4E-2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>-0.86399999999999999</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="6">
-        <v>-2.532</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E4" s="6">
-        <v>-1.2549999999999999</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="9">
-        <v>-3.2519999999999998</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="E5" s="9">
-        <v>-1.38</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5.524</v>
-      </c>
-      <c r="D6" s="5" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="8">
+        <v>6.2869999999999999</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="6">
-        <v>2.177</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="13">
-        <v>-2.81</v>
-      </c>
-      <c r="D7" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E7" s="13">
-        <v>-1.0529999999999999</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="E11" s="8">
+        <v>0.747</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1.417</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="E9" s="9">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F9" s="7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="15">
+        <v>6.0910000000000002</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="6">
-        <v>3.008</v>
-      </c>
-      <c r="D10" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1.47</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="9">
-        <v>6.2869999999999999</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.747</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="6">
-        <v>5.0199999999999996</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1.417</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="9">
-        <v>3.9550000000000001</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="16">
-        <v>6.0910000000000002</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="16">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3194,343 +3233,343 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4">
+        <v>-7.4450000000000003</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-6.1369999999999996</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="8">
+        <v>6.61</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.512</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.5920000000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.111</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="5">
-        <v>-7.4450000000000003</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C7" s="12">
+        <v>5.7110000000000003</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="5">
-        <v>-6.1369999999999996</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E7" s="12">
+        <v>4.524</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.5229999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.128</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.391</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3.3690000000000002</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2.7879999999999998</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5.3559999999999999</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="5">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="9">
-        <v>6.61</v>
-      </c>
-      <c r="D3" s="7" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.748</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5.415</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.72899999999999998</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.84</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E12" s="4">
+        <v>4.1710000000000003</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1.512</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="E5" s="9">
-        <v>1.2310000000000001</v>
-      </c>
-      <c r="F5" s="7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.4670000000000001</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1.5920000000000001</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.111</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1.42</v>
-      </c>
-      <c r="F6" s="5" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="13">
-        <v>5.7110000000000003</v>
-      </c>
-      <c r="D7" s="13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>5.444</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="13">
-        <v>4.524</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="E15" s="6">
+        <v>4.4710000000000001</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1.5229999999999999</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.128</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1.391</v>
-      </c>
-      <c r="F8" s="5" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4">
+        <v>-4.96</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="4">
+        <v>-3.161</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="17">
+        <v>-1.7749999999999999</v>
+      </c>
+      <c r="D17" s="17">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E17" s="17">
+        <v>-1.2010000000000001</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="7">
-        <v>3.3690000000000002</v>
-      </c>
-      <c r="D9" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="E9" s="7">
-        <v>2.7879999999999998</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="5">
-        <v>5.3559999999999999</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="6">
-        <v>4.2290000000000001</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0.748</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0.69699999999999995</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="5">
-        <v>5.415</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="5">
-        <v>4.1710000000000003</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1.4670000000000001</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1.0169999999999999</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0.66500000000000004</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.50600000000000001</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="7">
-        <v>5.444</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="7">
-        <v>4.4710000000000001</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="5">
-        <v>-4.96</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="5">
-        <v>-3.161</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="18">
-        <v>-1.7749999999999999</v>
-      </c>
-      <c r="D17" s="18">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="E17" s="18">
-        <v>-1.2010000000000001</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3542,359 +3581,359 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4062B321-D291-B042-BB06-2BF9F3E8430C}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="F17" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="9" style="19" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="19"/>
+    <col min="1" max="1" width="16.83203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="9" style="18" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>-6.7759999999999998</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>-2.7010000000000001</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>137</v>
+      <c r="F2" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-0.63800000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-0.26900000000000002</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2.492</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.84</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-1.2629999999999999</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-0.54400000000000004</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1.825</v>
+      </c>
+      <c r="D9" s="8">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.62</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3.1059999999999999</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.331</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2.5379999999999998</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.121</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.861</v>
+      </c>
+      <c r="D14" s="4">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="9">
-        <v>2.1880000000000002</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="F3" s="7" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4.4240000000000004</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6">
-        <v>-0.63800000000000001</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="E4" s="6">
-        <v>-0.26900000000000002</v>
-      </c>
-      <c r="F4" s="5" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3.3690000000000002</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2.492</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E5" s="9">
-        <v>1.0740000000000001</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1.1719999999999999</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0.84</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="6">
-        <v>-1.2629999999999999</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="E8" s="6">
-        <v>-0.54400000000000004</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1.825</v>
-      </c>
-      <c r="D9" s="9">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0.62</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="6">
-        <v>3.1059999999999999</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2E-3</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1.331</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="8" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="9">
-        <v>2.5379999999999998</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="6">
-        <v>1.2609999999999999</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.121</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1.861</v>
-      </c>
-      <c r="D14" s="5">
-        <v>6.3E-2</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1.1439999999999999</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="9">
-        <v>4.4240000000000004</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="B17" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="42">
+        <v>4.399</v>
+      </c>
+      <c r="D17" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="9">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="E17" s="42">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="F17" s="42" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="47">
-        <v>3.3690000000000002</v>
-      </c>
-      <c r="D16" s="47">
-        <v>1E-3</v>
-      </c>
-      <c r="E16" s="47">
-        <v>0.85</v>
-      </c>
-      <c r="F16" s="46" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="48">
-        <v>4.399</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="48">
-        <v>1.1180000000000001</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3921,343 +3960,343 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="50" t="s">
+      <c r="E1" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="44" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>2.3010000000000002</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>1.1200000000000001</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="8">
+        <v>-15.089</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="8">
+        <v>-0.73</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-0.76600000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-0.39600000000000002</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2.8860000000000001</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1.5229999999999999</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.6739999999999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2.0070000000000001</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.252</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.188</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.503</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3.032</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2.04</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="9">
-        <v>-15.089</v>
-      </c>
-      <c r="D3" s="9" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8">
+        <v>6.1280000000000001</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="9">
-        <v>-0.73</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6">
-        <v>-0.76600000000000001</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="E4" s="6">
-        <v>-0.39600000000000002</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2.8860000000000001</v>
-      </c>
-      <c r="D5" s="7">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E5" s="9">
-        <v>1.5229999999999999</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E15" s="8">
+        <v>1.67</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="6">
-        <v>2.6739999999999999</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2.0070000000000001</v>
-      </c>
-      <c r="F6" s="5" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3.8039999999999998</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1.163</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0.252</v>
-      </c>
-      <c r="F7" s="12" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="42">
+        <v>5.5830000000000002</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="42">
+        <v>1.7310000000000001</v>
+      </c>
+      <c r="F17" s="42" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.188</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D9" s="9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0.83199999999999996</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.503</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="9">
-        <v>3.032</v>
-      </c>
-      <c r="D11" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="E11" s="9">
-        <v>1.0880000000000001</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="6">
-        <v>2.04</v>
-      </c>
-      <c r="D12" s="5">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.253</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1.4930000000000001</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1.1240000000000001</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="9">
-        <v>6.1280000000000001</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="9">
-        <v>1.67</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="47">
-        <v>3.8039999999999998</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="47">
-        <v>1.163</v>
-      </c>
-      <c r="F16" s="46" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="48">
-        <v>5.5830000000000002</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="48">
-        <v>1.7310000000000001</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing supplemental table format
Made back transformation of effect sizes more clear and streamlined in the script
</commit_message>
<xml_diff>
--- a/supplements/Formatted Supplemental Tables.xlsx
+++ b/supplements/Formatted Supplemental Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahrempel/My Drive/Research_Archives/ecological_drivers_corallivory/supplements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BDCFCE-235A-2A48-8FE9-E9A6BAD7A301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6410B8AE-5A35-EB45-A86F-8488D5450D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="500" windowWidth="22540" windowHeight="16620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20500" yWindow="2100" windowWidth="22540" windowHeight="16620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_S1" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="163">
   <si>
     <t>Region</t>
   </si>
@@ -282,79 +282,25 @@
     <t>Transect depth (m)</t>
   </si>
   <si>
-    <t>[-2.212, -0.548]</t>
-  </si>
-  <si>
-    <t>[-0.437, 1.233]</t>
-  </si>
-  <si>
-    <t>[-0.069, 0.103]</t>
-  </si>
-  <si>
-    <t>[0.634, 1.236]</t>
-  </si>
-  <si>
-    <t>[0.514, 0.980]</t>
-  </si>
-  <si>
-    <t>[1.405, 2.950]</t>
-  </si>
-  <si>
-    <t>[-2.216, 0.723]</t>
-  </si>
-  <si>
-    <t>[0.512, 2.429]</t>
-  </si>
-  <si>
-    <t>[-1.874, 0.146]</t>
-  </si>
-  <si>
-    <t>[-2.227, -0.284]</t>
-  </si>
-  <si>
-    <t>[-1.788, -0.319]</t>
-  </si>
-  <si>
-    <t>[0.864, 1.970]</t>
-  </si>
-  <si>
-    <t>[0.283, 0.840]</t>
-  </si>
-  <si>
     <t>[-7.752, -4.521]</t>
   </si>
   <si>
     <t>[-1.418, 3.098]</t>
   </si>
   <si>
-    <t>[-0.365, 2.826]</t>
-  </si>
-  <si>
     <t>[-0.328, 3.167]</t>
   </si>
   <si>
-    <t>[2.972, 6.077]</t>
-  </si>
-  <si>
     <t>[-0.399, 3.181]</t>
   </si>
   <si>
-    <t>[1.166, 4.409]</t>
-  </si>
-  <si>
     <t>[2.681, 5.776]</t>
   </si>
   <si>
-    <t>[2.662, 5.681]</t>
-  </si>
-  <si>
     <t>[-0.342, 2.376]</t>
   </si>
   <si>
     <t>[-1.276, 2.586]</t>
-  </si>
-  <si>
-    <t>[2.861, 6.081]</t>
   </si>
   <si>
     <t>[-2.527, 0.125]</t>
@@ -505,21 +451,6 @@
         <family val="1"/>
       </rPr>
       <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Proportion of total observed predation (%)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>  </t>
     </r>
   </si>
   <si>
@@ -572,102 +503,6 @@
     <t>Area predated (%)</t>
   </si>
   <si>
-    <t>[-0.061, 2.348]</t>
-  </si>
-  <si>
-    <t>[0.009, 0.165]</t>
-  </si>
-  <si>
-    <t>[-1.097, 0.558]</t>
-  </si>
-  <si>
-    <t>[0.229, 1.919]</t>
-  </si>
-  <si>
-    <t>[-0.891, 1.095]</t>
-  </si>
-  <si>
-    <t>[-0.046, 1.286]</t>
-  </si>
-  <si>
-    <t>[0.491, 2.171]</t>
-  </si>
-  <si>
-    <t>[-0.213, 0.983]</t>
-  </si>
-  <si>
-    <t>[0.549, 1.423]</t>
-  </si>
-  <si>
-    <t>[0.356, 1.345]</t>
-  </si>
-  <si>
-    <t>[-3.482, -1.920]</t>
-  </si>
-  <si>
-    <t>[-0.483, 1.920]</t>
-  </si>
-  <si>
-    <t>[-1.387, 0.300]</t>
-  </si>
-  <si>
-    <t>[0.170, 1.319]</t>
-  </si>
-  <si>
-    <t>[-0.460, 0.702]</t>
-  </si>
-  <si>
-    <t>[0.620, 1.616]</t>
-  </si>
-  <si>
-    <t>[0.166, 2.075]</t>
-  </si>
-  <si>
-    <t>[-0.825, -0.635]</t>
-  </si>
-  <si>
-    <t>[0.489, 2.557]</t>
-  </si>
-  <si>
-    <t>[0.536, 3.479]</t>
-  </si>
-  <si>
-    <t>[-0.963, 1.468]</t>
-  </si>
-  <si>
-    <t>[0.019, 1.645]</t>
-  </si>
-  <si>
-    <t>[0.385, 1.792]</t>
-  </si>
-  <si>
-    <t>[-0.459, 0.965]</t>
-  </si>
-  <si>
-    <t>[-0.351, 2.598]</t>
-  </si>
-  <si>
-    <t>[1.136, 2.204]</t>
-  </si>
-  <si>
-    <t>[0.564, 1.762]</t>
-  </si>
-  <si>
-    <t>[1.123, 2.339]</t>
-  </si>
-  <si>
-    <t>[-1.410, 0.618]</t>
-  </si>
-  <si>
-    <t>[-0.845, 1.220]</t>
-  </si>
-  <si>
-    <t>[-0.525, 1.530]</t>
-  </si>
-  <si>
-    <t>[0.030, 1.493]</t>
-  </si>
-  <si>
     <t>[-1.295, 2.937]</t>
   </si>
   <si>
@@ -680,12 +515,6 @@
     <t>[-0.029, 0.011]</t>
   </si>
   <si>
-    <t>[-7.703, -3.274]</t>
-  </si>
-  <si>
-    <t>[0.048, 0.785]</t>
-  </si>
-  <si>
     <t>[-0.061, 0.075]</t>
   </si>
   <si>
@@ -696,6 +525,181 @@
   </si>
   <si>
     <t>√(Corallivore density) x (coral cover)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>[-7.700, -3.273]</t>
+  </si>
+  <si>
+    <t>[0.048, 0.784]</t>
+  </si>
+  <si>
+    <r>
+      <t>Proportion of total observed predation (%)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>  </t>
+    </r>
+  </si>
+  <si>
+    <t>[-2.278, 0.751]</t>
+  </si>
+  <si>
+    <t>[0.493, 2.443]</t>
+  </si>
+  <si>
+    <t>[-1.841, 0.368]</t>
+  </si>
+  <si>
+    <t>[-2.26, -0.103]</t>
+  </si>
+  <si>
+    <t>[-2.405, -0.463]</t>
+  </si>
+  <si>
+    <t>[-0.066, 0.108]</t>
+  </si>
+  <si>
+    <t>[-1.821, -0.308]</t>
+  </si>
+  <si>
+    <t>[-0.464, 1.244]</t>
+  </si>
+  <si>
+    <t>[0.492, 1.005]</t>
+  </si>
+  <si>
+    <t>[0.888, 2.093]</t>
+  </si>
+  <si>
+    <t>[0.277, 0.887]</t>
+  </si>
+  <si>
+    <t>[0.604, 1.278]</t>
+  </si>
+  <si>
+    <t>[1.430, 3.015]</t>
+  </si>
+  <si>
+    <t>[-0.365, 2.827]</t>
+  </si>
+  <si>
+    <t>[2.662, 5.682]</t>
+  </si>
+  <si>
+    <t>[2.970, 6.076]</t>
+  </si>
+  <si>
+    <t>[1.167, 4.410]</t>
+  </si>
+  <si>
+    <t>[2.861, 6.080]</t>
+  </si>
+  <si>
+    <t>[0.233, 2.066]</t>
+  </si>
+  <si>
+    <t>[-0.826, -0.644]</t>
+  </si>
+  <si>
+    <t>[-1.372, 0.575]</t>
+  </si>
+  <si>
+    <t>[0.538, 2.524]</t>
+  </si>
+  <si>
+    <t>[0.576, 3.401]</t>
+  </si>
+  <si>
+    <t>[-0.905, 1.429]</t>
+  </si>
+  <si>
+    <t>[-0.824, 1.158]</t>
+  </si>
+  <si>
+    <t>[0.015, 1.576]</t>
+  </si>
+  <si>
+    <t>[-0.473, 1.501]</t>
+  </si>
+  <si>
+    <t>[0.421, 1.772]</t>
+  </si>
+  <si>
+    <t>[0.058, 1.463]</t>
+  </si>
+  <si>
+    <t>[-0.424, 0.942]</t>
+  </si>
+  <si>
+    <t>[1.148, 2.174]</t>
+  </si>
+  <si>
+    <t>[1.166, 2.333]</t>
+  </si>
+  <si>
+    <t>[-0.302, 2.530]</t>
+  </si>
+  <si>
+    <t>[0.670, 1.821]</t>
+  </si>
+  <si>
+    <t>[-3.537, -1.824]</t>
+  </si>
+  <si>
+    <t>[0.008, 0.175]</t>
+  </si>
+  <si>
+    <t>[0.039, 1.984]</t>
+  </si>
+  <si>
+    <t>[-0.602, 1.989]</t>
+  </si>
+  <si>
+    <t>[-1.156, 1.178]</t>
+  </si>
+  <si>
+    <t>[-1.517, 0.367]</t>
+  </si>
+  <si>
+    <t>[-0.192, 1.552]</t>
+  </si>
+  <si>
+    <t>[0.179, 2.277]</t>
+  </si>
+  <si>
+    <t>[0.022, 1.357]</t>
+  </si>
+  <si>
+    <t>[-0.372, 1.058]</t>
+  </si>
+  <si>
+    <t>[-0.546, 0.745]</t>
+  </si>
+  <si>
+    <t>[-0.244, 2.418]</t>
+  </si>
+  <si>
+    <t>[0.466, 1.465]</t>
+  </si>
+  <si>
+    <t>[0.101, 1.335]</t>
+  </si>
+  <si>
+    <t>[0.527, 1.766]</t>
+  </si>
+  <si>
+    <t>[-1.204, 0.600]</t>
   </si>
 </sst>
 </file>
@@ -707,7 +711,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -889,8 +893,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1079,6 +1105,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,17 +1324,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1349,9 +1375,6 @@
     <xf numFmtId="2" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1370,9 +1393,6 @@
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1418,31 +1438,31 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1809,7 +1829,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1821,542 +1841,542 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="44" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="29">
         <v>9.2684440000000006</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="29">
         <v>-82.241917000000001</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="18">
         <v>2</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="30">
         <v>9.3594439999999999</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="30">
         <v>-82.276667000000003</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>2</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="29">
         <v>9.2147780000000008</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="29">
         <v>-82.324556000000001</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="18">
         <v>2</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="30">
         <v>9.2438330000000004</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="30">
         <v>-82.145139</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="9">
         <v>2</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="29">
         <v>9.2883060000000004</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="29">
         <v>-82.256777999999997</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="18">
         <v>2</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="30">
         <v>9.2346939999999993</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="30">
         <v>-82.345528000000002</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="29">
         <v>9.24</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="29">
         <v>-82.337500000000006</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="18">
         <v>2</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="30">
         <v>9.2712500000000002</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="30">
         <v>-82.298056000000003</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="9">
         <v>2</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="29">
         <v>9.3488059999999997</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="29">
         <v>-82.262861000000001</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="18">
         <v>2</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="32">
         <v>9.2891940000000002</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="32">
         <v>-82.295693999999997</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="31">
         <v>2</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="29">
         <v>24.961189999999998</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="29">
         <v>-80.456647000000004</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="18">
         <v>2</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="33">
         <v>24.927060000000001</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="33">
         <v>-80.505504999999999</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="26">
         <v>3</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="26">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="29">
         <v>25.03482</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="29">
         <v>-80.347778000000005</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="18">
         <v>4</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="35">
         <v>25.008469999999999</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="35">
         <v>-80.376266000000001</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="34">
         <v>2</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C16" s="29">
         <v>17.787870000000002</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="29">
         <v>-64.609954999999999</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="18">
         <v>11</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="30">
         <v>17.786709999999999</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="30">
         <v>-64.608797999999993</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="9">
         <v>23</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="29">
         <v>17.789390000000001</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="29">
         <v>-64.610279000000006</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="18">
         <v>8</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="30">
         <v>17.77308</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="30">
         <v>-64.812824000000006</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="9">
         <v>32</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="9">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="29">
         <v>17.761479999999999</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="29">
         <v>-64.720011999999997</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="18">
         <v>30</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="18">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="30">
         <v>17.768439999999998</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="30">
         <v>-64.823126000000002</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="9">
         <v>27</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="29">
         <v>17.779879999999999</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="29">
         <v>-64.760394000000005</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="18">
         <v>19</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="18">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="32">
         <v>17.761119999999998</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="32">
         <v>-64.607426000000004</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="31">
         <v>25</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="33">
+      <c r="C24" s="29">
         <v>12.125730000000001</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="29">
         <v>-68.288225999999995</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="18">
         <v>7</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="33">
         <v>12.17428</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="33">
         <v>-68.290726000000006</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="26">
         <v>5</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="26">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="29">
         <v>12.21912</v>
       </c>
-      <c r="D26" s="33">
+      <c r="D26" s="29">
         <v>-68.352683999999996</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="18">
         <v>26</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="37">
         <v>12.21496</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="37">
         <v>-68.337958</v>
       </c>
-      <c r="E27" s="40">
+      <c r="E27" s="36">
         <v>32</v>
       </c>
-      <c r="F27" s="40">
+      <c r="F27" s="36">
         <v>8</v>
       </c>
     </row>
@@ -2367,10 +2387,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FD2E0D-B2A3-4944-B56F-94C4BD8802C5}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="A1:C16"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2380,186 +2400,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>115</v>
+      <c r="C1" s="44" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="21">
+      <c r="A2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="18">
         <v>74</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="24">
         <v>22.6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>73</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>22.3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="18">
         <v>59</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>57</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>17.399999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="18">
         <v>12</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>3.7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>11</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>3.4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="18">
         <v>9</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>2.8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>9</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>2.8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="18">
         <v>8</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>2.4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="18">
         <v>3</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="18">
         <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="26">
         <v>3</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="26">
         <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="18">
         <v>2</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="18">
         <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="26">
         <v>1</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="26">
         <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="28">
         <v>1</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="28">
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2571,7 +2596,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="A1:C11"/>
+      <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2582,123 +2607,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="43" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="18">
         <v>2.38</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>1.85</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="18">
         <v>1.02</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>0.92</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="18">
         <v>0.37</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>0.26</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="18">
         <v>0.02</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>0</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="20">
         <v>0</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="22">
         <v>0</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="23">
         <v>45</v>
       </c>
     </row>
@@ -2711,8 +2736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1162ECB6-7014-2547-9AF5-E86990302D6E}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2727,183 +2752,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="50">
+      <c r="C2" s="3">
         <v>0.76</v>
       </c>
-      <c r="D2" s="50">
+      <c r="D2" s="3">
         <v>0.44700000000000001</v>
       </c>
-      <c r="E2" s="50">
+      <c r="E2" s="3">
         <v>0.82099999999999995</v>
       </c>
-      <c r="F2" s="49" t="s">
-        <v>152</v>
+      <c r="F2" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="48">
+      <c r="B3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="6">
         <v>1.1990000000000001</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="6">
         <v>0.23</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="6">
         <v>0.21099999999999999</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>153</v>
+      <c r="F3" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="39">
         <v>-0.36299999999999999</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="39">
         <v>0.71599999999999997</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="39">
         <v>-1.2E-2</v>
       </c>
-      <c r="F4" s="45" t="s">
-        <v>154</v>
+      <c r="F4" s="18" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="51">
+      <c r="B5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="40">
         <v>-0.84799999999999998</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="40">
         <v>0.39700000000000002</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="40">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="F5" s="42" t="s">
-        <v>155</v>
+      <c r="F5" s="38" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="49" t="s">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="50">
-        <v>-4.859</v>
-      </c>
-      <c r="D6" s="50" t="s">
+      <c r="C6" s="3">
+        <v>-4.8579999999999997</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="50">
-        <v>-5.4880000000000004</v>
-      </c>
-      <c r="F6" s="49" t="s">
-        <v>156</v>
+      <c r="E6" s="3">
+        <v>-5.4859999999999998</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="48">
-        <v>2.2160000000000002</v>
-      </c>
-      <c r="D7" s="48">
+      <c r="A7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2.2170000000000001</v>
+      </c>
+      <c r="D7" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="E7" s="48">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="F7" s="47" t="s">
-        <v>157</v>
+      <c r="E7" s="6">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="49" t="s">
+      <c r="A8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="49">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="D8" s="49">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="E8" s="49">
+      <c r="C8" s="2">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="E8" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F8" s="49" t="s">
-        <v>158</v>
+      <c r="F8" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="51">
-        <v>-0.54700000000000004</v>
-      </c>
-      <c r="D9" s="51">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="E9" s="51">
+      <c r="A9" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="40">
+        <v>-0.54600000000000004</v>
+      </c>
+      <c r="D9" s="40">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="E9" s="40">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F9" s="42" t="s">
-        <v>159</v>
+      <c r="F9" s="38" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2916,7 +2941,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F14" sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2930,283 +2955,283 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="46" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-0.98799999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-0.76400000000000001</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6">
+        <v>-1.3069999999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.191</v>
+      </c>
+      <c r="E3" s="6">
+        <v>-0.73699999999999999</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-2.1469999999999998</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-1.181</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-2.8940000000000001</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>-1.4339999999999999</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.4950000000000001</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.222</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-2.7570000000000001</v>
+      </c>
+      <c r="D7" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E7" s="10">
+        <v>-1.0640000000000001</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="5">
-        <v>-0.996</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="E2" s="5">
-        <v>-0.746</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="8">
-        <v>-1.6759999999999999</v>
-      </c>
-      <c r="D3" s="6">
-        <v>9.4E-2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>-0.86399999999999999</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="5">
-        <v>-2.532</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E4" s="5">
-        <v>-1.2549999999999999</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="8">
-        <v>-3.2519999999999998</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="E5" s="8">
-        <v>-1.38</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>5.524</v>
-      </c>
-      <c r="D6" s="4" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2.9510000000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.468</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5.7220000000000004</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="5">
-        <v>2.177</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="12">
-        <v>-2.81</v>
-      </c>
-      <c r="D7" s="6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E7" s="12">
-        <v>-1.0529999999999999</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.35</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="E9" s="8">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3.008</v>
-      </c>
-      <c r="D10" s="4">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1.47</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="8">
-        <v>6.2869999999999999</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6">
+        <v>0.748</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="8">
-        <v>0.747</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="5">
-        <v>5.0199999999999996</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="3">
+        <v>1.4910000000000001</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3.7440000000000002</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="5">
-        <v>1.417</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="8">
-        <v>3.9550000000000001</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="6">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="13">
+        <v>5.48</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="8">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="15">
-        <v>6.0910000000000002</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>83</v>
+      <c r="E14" s="13">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3233,343 +3258,343 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="46" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="4">
-        <v>-7.4450000000000003</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="2">
+        <v>-7.444</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>-6.1369999999999996</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>93</v>
+      <c r="F2" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="8">
-        <v>6.61</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="6">
+        <v>6.6120000000000001</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>1E-3</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>106</v>
+      <c r="F3" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>0.72899999999999998</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0.46600000000000003</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>0.84</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>94</v>
+      <c r="F4" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>1.512</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>0.13100000000000001</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>1.2310000000000001</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>95</v>
+      <c r="F5" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>1.5920000000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>0.111</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>1.42</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>96</v>
+      <c r="F6" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="12">
-        <v>5.7110000000000003</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="10">
+        <v>5.71</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="12">
-        <v>4.524</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>97</v>
+      <c r="E7" s="10">
+        <v>4.5229999999999997</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>1.5229999999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>0.128</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>1.391</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>98</v>
+      <c r="F8" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="6">
-        <v>3.3690000000000002</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="C9" s="4">
+        <v>3.37</v>
+      </c>
+      <c r="D9" s="4">
         <v>1E-3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>2.7879999999999998</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>99</v>
+      <c r="F9" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="4">
-        <v>5.3559999999999999</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="2">
+        <v>5.3550000000000004</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="5">
-        <v>4.2290000000000001</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>100</v>
+      <c r="E10" s="3">
+        <v>4.2279999999999998</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="8">
-        <v>0.748</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="C11" s="6">
+        <v>0.747</v>
+      </c>
+      <c r="D11" s="6">
         <v>0.45500000000000002</v>
       </c>
-      <c r="E11" s="6">
-        <v>0.69699999999999995</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>107</v>
+      <c r="E11" s="4">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>5.415</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="4">
-        <v>4.1710000000000003</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>101</v>
+      <c r="E12" s="2">
+        <v>4.1719999999999997</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="6">
-        <v>1.4670000000000001</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="C13" s="4">
+        <v>1.466</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E13" s="4">
         <v>1.0169999999999999</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>102</v>
+      <c r="F13" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>0.66500000000000004</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>0.50600000000000001</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>103</v>
+      <c r="F14" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>5.444</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>4.4710000000000001</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>104</v>
+      <c r="F15" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="2">
         <v>-4.96</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <v>-3.161</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>108</v>
+      <c r="F16" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="17">
-        <v>-1.7749999999999999</v>
-      </c>
-      <c r="D17" s="17">
+      <c r="C17" s="15">
+        <v>-1.776</v>
+      </c>
+      <c r="D17" s="15">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="15">
         <v>-1.2010000000000001</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>105</v>
+      <c r="F17" s="15" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3581,359 +3606,359 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4062B321-D291-B042-BB06-2BF9F3E8430C}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="9" style="18" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="18"/>
+    <col min="1" max="1" width="16.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="9" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="16" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="46" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="5">
-        <v>-6.7759999999999998</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3">
+        <v>-6.1349999999999998</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="5">
-        <v>-2.7010000000000001</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>130</v>
+      <c r="E2" s="3">
+        <v>-2.681</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="8">
-        <v>2.1880000000000002</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>121</v>
+      <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.145</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="5">
-        <v>-0.63800000000000001</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="E4" s="5">
-        <v>-0.26900000000000002</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>122</v>
+      <c r="C4" s="3">
+        <v>-0.65700000000000003</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-0.30199999999999999</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="8">
-        <v>2.492</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1.0740000000000001</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>123</v>
+      <c r="C5" s="6">
+        <v>2.0379999999999998</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.012</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="5">
-        <v>1.1719999999999999</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>131</v>
+      <c r="C6" s="3">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="12">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>124</v>
+      <c r="C7" s="10">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="5">
-        <v>-1.2629999999999999</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="E8" s="5">
-        <v>-0.54400000000000004</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>132</v>
+      <c r="C8" s="3">
+        <v>-1.1970000000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-0.57499999999999996</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="8">
-        <v>1.825</v>
-      </c>
-      <c r="D9" s="8">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.62</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>125</v>
+      <c r="C9" s="6">
+        <v>1.528</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.127</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="5">
-        <v>3.1059999999999999</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2E-3</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1.331</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>126</v>
+      <c r="C10" s="3">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.228</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="8">
-        <v>2.5379999999999998</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>133</v>
+      <c r="C11" s="6">
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="5">
-        <v>1.2609999999999999</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>127</v>
+      <c r="C12" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="8">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.121</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>134</v>
+      <c r="C13" s="6">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="E13" s="6">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="5">
-        <v>1.861</v>
-      </c>
-      <c r="D14" s="4">
-        <v>6.3E-2</v>
-      </c>
-      <c r="E14" s="5">
-        <v>1.1439999999999999</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>120</v>
+      <c r="C14" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.087</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="8">
-        <v>4.4240000000000004</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="6">
+        <v>3.7879999999999998</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="8">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>128</v>
+      <c r="E15" s="6">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="5">
-        <v>3.3690000000000002</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0.85</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>129</v>
+      <c r="C16" s="3">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="42">
-        <v>4.399</v>
-      </c>
-      <c r="D17" s="42" t="s">
+      <c r="C17" s="38">
+        <v>3.6280000000000001</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="42">
-        <v>1.1180000000000001</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>135</v>
+      <c r="E17" s="38">
+        <v>1.147</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3946,7 +3971,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="A1:F17"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3960,343 +3985,343 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="5">
-        <v>2.3010000000000002</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="3">
+        <v>2.4580000000000002</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.149</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="6">
+        <v>-15.835000000000001</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="6">
+        <v>-0.73499999999999999</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-0.80200000000000005</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-0.39800000000000002</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3.0219999999999998</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.5309999999999999</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.7589999999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="8">
-        <v>-15.089</v>
-      </c>
-      <c r="D3" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.998</v>
+      </c>
+      <c r="D9" s="6">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.307</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3.181</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.121</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.542</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.123</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>6.3490000000000002</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="8">
-        <v>-0.73</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="5">
-        <v>-0.76600000000000001</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="E4" s="5">
-        <v>-0.39600000000000002</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="8">
-        <v>2.8860000000000001</v>
-      </c>
-      <c r="D5" s="6">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1.5229999999999999</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2.6739999999999999</v>
-      </c>
-      <c r="D6" s="4">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E6" s="5">
-        <v>2.0070000000000001</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0.252</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.188</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="8">
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D9" s="8">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.83199999999999996</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.503</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="8">
-        <v>3.032</v>
-      </c>
-      <c r="D11" s="8">
-        <v>2E-3</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1.0880000000000001</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2.04</v>
-      </c>
-      <c r="D12" s="4">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.253</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E15" s="6">
+        <v>1.661</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1.4930000000000001</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="E14" s="5">
-        <v>1.1240000000000001</v>
-      </c>
-      <c r="F14" s="4" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4.2439999999999998</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.246</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="38">
+        <v>5.8769999999999998</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="38">
+        <v>1.75</v>
+      </c>
+      <c r="F17" s="38" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="8">
-        <v>6.1280000000000001</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="8">
-        <v>1.67</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="5">
-        <v>3.8039999999999998</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="5">
-        <v>1.163</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="42">
-        <v>5.5830000000000002</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="42">
-        <v>1.7310000000000001</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>